<commit_message>
Operations with stocks and derivatives were segregated in russian 3-NDFL tax report form (Closed #8)
</commit_message>
<xml_diff>
--- a/docs/ru-tax-3ndfl/3ndfl_tax_report.xlsx
+++ b/docs/ru-tax-3ndfl/3ndfl_tax_report.xlsx
@@ -8,16 +8,17 @@
   </bookViews>
   <sheets>
     <sheet name="Дивиденды" sheetId="1" r:id="rId1"/>
-    <sheet name="Сделки" sheetId="2" r:id="rId2"/>
-    <sheet name="Комиссии" sheetId="3" r:id="rId3"/>
-    <sheet name="Корп.события" sheetId="4" r:id="rId4"/>
+    <sheet name="Сделки с ЦБ" sheetId="2" r:id="rId2"/>
+    <sheet name="Сделки с ПФИ" sheetId="3" r:id="rId3"/>
+    <sheet name="Комиссии" sheetId="4" r:id="rId4"/>
+    <sheet name="Корп.события" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="104">
   <si>
     <t>Отчет по дивидендам, полученным в отчетном периоде</t>
   </si>
@@ -199,21 +200,51 @@
     <t>(16)</t>
   </si>
   <si>
+    <t>VLO</t>
+  </si>
+  <si>
+    <t>Покупка</t>
+  </si>
+  <si>
+    <t>24.07.2020</t>
+  </si>
+  <si>
+    <t>Продажа</t>
+  </si>
+  <si>
+    <t>29.07.2020</t>
+  </si>
+  <si>
+    <t>31.07.2020</t>
+  </si>
+  <si>
+    <t>FB</t>
+  </si>
+  <si>
+    <t>25.08.2020</t>
+  </si>
+  <si>
+    <t>27.08.2020</t>
+  </si>
+  <si>
+    <t>Отчет по сделкам с производными финансовыми инструментами, завершённым в отчетном периоде</t>
+  </si>
+  <si>
+    <t>Доход, RUB (код 1532)</t>
+  </si>
+  <si>
+    <t>Расход, RUB (код 206)</t>
+  </si>
+  <si>
     <t>AAL   210115C00030000</t>
   </si>
   <si>
-    <t>Продажа</t>
-  </si>
-  <si>
     <t>15.01.2020</t>
   </si>
   <si>
     <t>16.01.2020</t>
   </si>
   <si>
-    <t>Покупка</t>
-  </si>
-  <si>
     <t>28.02.2020</t>
   </si>
   <si>
@@ -227,27 +258,6 @@
   </si>
   <si>
     <t>22.06.2020</t>
-  </si>
-  <si>
-    <t>24.07.2020</t>
-  </si>
-  <si>
-    <t>VLO</t>
-  </si>
-  <si>
-    <t>29.07.2020</t>
-  </si>
-  <si>
-    <t>31.07.2020</t>
-  </si>
-  <si>
-    <t>FB</t>
-  </si>
-  <si>
-    <t>25.08.2020</t>
-  </si>
-  <si>
-    <t>27.08.2020</t>
   </si>
   <si>
     <t>Отчет по комиссиям, уплаченным брокеру в отчетном периоде</t>
@@ -997,7 +1007,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P18"/>
+  <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1160,74 +1170,74 @@
         <v>62</v>
       </c>
       <c r="E10" s="7">
-        <v>61.414</v>
+        <v>70.7881</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G10" s="7">
-        <v>61.414</v>
+        <v>70.7881</v>
       </c>
       <c r="H10" s="11">
-        <v>2.94</v>
+        <v>64</v>
       </c>
       <c r="I10" s="8">
-        <v>294</v>
+        <v>6400</v>
       </c>
       <c r="J10" s="8">
-        <v>18055.72</v>
+        <v>453043.84</v>
       </c>
       <c r="K10" s="11">
-        <v>0.8018858</v>
+        <v>0</v>
       </c>
       <c r="L10" s="8">
-        <v>49.25</v>
+        <v>0</v>
       </c>
       <c r="M10" s="8">
-        <v>18055.72</v>
+        <v>424325.64</v>
       </c>
       <c r="N10" s="8">
-        <v>8717.390000000001</v>
+        <v>453141.36</v>
       </c>
       <c r="O10" s="8">
-        <v>9338.33</v>
+        <v>-28815.72000000003</v>
       </c>
       <c r="P10" s="8">
-        <v>161.1043142</v>
+        <v>-501.3500000000004</v>
       </c>
     </row>
     <row r="11" spans="1:16">
       <c r="A11" s="6"/>
       <c r="B11" s="10"/>
       <c r="C11" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="E11" s="7">
+        <v>72.23480000000001</v>
+      </c>
+      <c r="F11" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="E11" s="7">
-        <v>66.9909</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>66</v>
-      </c>
       <c r="G11" s="7">
-        <v>65.6097</v>
+        <v>71.9196</v>
       </c>
       <c r="H11" s="11">
-        <v>1.31</v>
+        <v>59</v>
       </c>
       <c r="I11" s="8">
-        <v>131</v>
+        <v>5900</v>
       </c>
       <c r="J11" s="8">
-        <v>8594.870000000001</v>
+        <v>424325.64</v>
       </c>
       <c r="K11" s="11">
-        <v>1.0938</v>
+        <v>1.35</v>
       </c>
       <c r="L11" s="8">
-        <v>73.27</v>
+        <v>97.52</v>
       </c>
       <c r="M11" s="8"/>
       <c r="N11" s="8"/>
@@ -1236,86 +1246,86 @@
     </row>
     <row r="12" spans="1:16">
       <c r="A12" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B12" s="12">
-        <v>100</v>
+        <v>11</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>61</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>68</v>
+        <v>35</v>
       </c>
       <c r="E12" s="4">
-        <v>69.57250000000001</v>
+        <v>71.58499999999999</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G12" s="4">
-        <v>69.61799999999999</v>
+        <v>71.59739999999999</v>
       </c>
       <c r="H12" s="13">
-        <v>4.54</v>
+        <v>232.11</v>
       </c>
       <c r="I12" s="5">
-        <v>454</v>
+        <v>2553.21</v>
       </c>
       <c r="J12" s="5">
-        <v>31606.57</v>
+        <v>182803.2</v>
       </c>
       <c r="K12" s="13">
-        <v>1.1058334</v>
+        <v>0.35</v>
       </c>
       <c r="L12" s="5">
-        <v>76.94</v>
+        <v>25.05</v>
       </c>
       <c r="M12" s="5">
-        <v>31606.57</v>
+        <v>245580.72</v>
       </c>
       <c r="N12" s="5">
-        <v>76.94</v>
+        <v>182854.33</v>
       </c>
       <c r="O12" s="5">
-        <v>31529.63</v>
+        <v>62726.39000000001</v>
       </c>
       <c r="P12" s="5">
-        <v>452.8941666</v>
+        <v>746.0900000000001</v>
       </c>
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="3"/>
       <c r="B13" s="12"/>
       <c r="C13" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E13" s="4">
-        <v>71.59739999999999</v>
+        <v>74.51260000000001</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="G13" s="4">
-        <v>70.96299999999999</v>
+        <v>74.41840000000001</v>
       </c>
       <c r="H13" s="13">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="I13" s="5">
-        <v>0</v>
+        <v>3300</v>
       </c>
       <c r="J13" s="5">
-        <v>0</v>
+        <v>245580.72</v>
       </c>
       <c r="K13" s="13">
-        <v>0</v>
+        <v>0.35</v>
       </c>
       <c r="L13" s="5">
-        <v>0</v>
+        <v>26.08</v>
       </c>
       <c r="M13" s="5"/>
       <c r="N13" s="5"/>
@@ -1323,204 +1333,28 @@
       <c r="P13" s="5"/>
     </row>
     <row r="14" spans="1:16">
-      <c r="A14" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="B14" s="10">
-        <v>100</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="E14" s="7">
-        <v>70.7881</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="G14" s="7">
-        <v>70.7881</v>
-      </c>
-      <c r="H14" s="11">
-        <v>64</v>
-      </c>
-      <c r="I14" s="8">
-        <v>6400</v>
-      </c>
-      <c r="J14" s="8">
-        <v>453043.84</v>
-      </c>
-      <c r="K14" s="11">
-        <v>0</v>
-      </c>
-      <c r="L14" s="8">
-        <v>0</v>
-      </c>
-      <c r="M14" s="8">
-        <v>424325.64</v>
-      </c>
-      <c r="N14" s="8">
-        <v>453141.36</v>
-      </c>
-      <c r="O14" s="8">
-        <v>-28815.72000000003</v>
-      </c>
-      <c r="P14" s="8">
-        <v>-501.3500000000004</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16">
-      <c r="A15" s="6"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="E15" s="7">
-        <v>72.23480000000001</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="G15" s="7">
-        <v>71.9196</v>
-      </c>
-      <c r="H15" s="11">
-        <v>59</v>
-      </c>
-      <c r="I15" s="8">
-        <v>5900</v>
-      </c>
-      <c r="J15" s="8">
-        <v>424325.64</v>
-      </c>
-      <c r="K15" s="11">
-        <v>1.35</v>
-      </c>
-      <c r="L15" s="8">
-        <v>97.52</v>
-      </c>
-      <c r="M15" s="8"/>
-      <c r="N15" s="8"/>
-      <c r="O15" s="8"/>
-      <c r="P15" s="8"/>
-    </row>
-    <row r="16" spans="1:16">
-      <c r="A16" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B16" s="12">
-        <v>11</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E16" s="4">
-        <v>71.58499999999999</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G16" s="4">
-        <v>71.59739999999999</v>
-      </c>
-      <c r="H16" s="13">
-        <v>232.11</v>
-      </c>
-      <c r="I16" s="5">
-        <v>2553.21</v>
-      </c>
-      <c r="J16" s="5">
-        <v>182803.2</v>
-      </c>
-      <c r="K16" s="13">
-        <v>0.35</v>
-      </c>
-      <c r="L16" s="5">
-        <v>25.05</v>
-      </c>
-      <c r="M16" s="5">
-        <v>245580.72</v>
-      </c>
-      <c r="N16" s="5">
-        <v>182854.33</v>
-      </c>
-      <c r="O16" s="5">
-        <v>62726.39000000001</v>
-      </c>
-      <c r="P16" s="5">
-        <v>746.0900000000001</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16">
-      <c r="A17" s="3"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="E17" s="4">
-        <v>74.51260000000001</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="G17" s="4">
-        <v>74.41840000000001</v>
-      </c>
-      <c r="H17" s="13">
-        <v>300</v>
-      </c>
-      <c r="I17" s="5">
-        <v>3300</v>
-      </c>
-      <c r="J17" s="5">
-        <v>245580.72</v>
-      </c>
-      <c r="K17" s="13">
-        <v>0.35</v>
-      </c>
-      <c r="L17" s="5">
-        <v>26.08</v>
-      </c>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="5"/>
-      <c r="P17" s="5"/>
-    </row>
-    <row r="18" spans="1:16">
-      <c r="L18" s="9" t="s">
+      <c r="L14" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="M18" s="9">
-        <f>SUM(M10:M17)</f>
-        <v>0</v>
-      </c>
-      <c r="N18" s="9">
-        <f>SUM(N10:N17)</f>
-        <v>0</v>
-      </c>
-      <c r="O18" s="9">
-        <f>SUM(O10:O17)</f>
-        <v>0</v>
-      </c>
-      <c r="P18" s="9">
-        <f>SUM(P10:P17)</f>
+      <c r="M14" s="9">
+        <f>SUM(M10:M13)</f>
+        <v>0</v>
+      </c>
+      <c r="N14" s="9">
+        <f>SUM(N10:N13)</f>
+        <v>0</v>
+      </c>
+      <c r="O14" s="9">
+        <f>SUM(O10:O13)</f>
+        <v>0</v>
+      </c>
+      <c r="P14" s="9">
+        <f>SUM(P10:P13)</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="12">
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="M10:M11"/>
@@ -1533,24 +1367,379 @@
     <mergeCell ref="N12:N13"/>
     <mergeCell ref="O12:O13"/>
     <mergeCell ref="P12:P13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="M14:M15"/>
-    <mergeCell ref="N14:N15"/>
-    <mergeCell ref="O14:O15"/>
-    <mergeCell ref="P14:P15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="M16:M17"/>
-    <mergeCell ref="N16:N17"/>
-    <mergeCell ref="O16:O17"/>
-    <mergeCell ref="P16:P17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:P14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="22.7109375" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" customWidth="1"/>
+    <col min="12" max="12" width="9.7109375" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" customWidth="1"/>
+    <col min="14" max="14" width="12.7109375" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" customWidth="1"/>
+    <col min="16" max="16" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="A1" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="60" customHeight="1">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" s="10">
+        <v>100</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" s="7">
+        <v>61.414</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="G10" s="7">
+        <v>61.414</v>
+      </c>
+      <c r="H10" s="11">
+        <v>2.94</v>
+      </c>
+      <c r="I10" s="8">
+        <v>294</v>
+      </c>
+      <c r="J10" s="8">
+        <v>18055.72</v>
+      </c>
+      <c r="K10" s="11">
+        <v>0.8018858</v>
+      </c>
+      <c r="L10" s="8">
+        <v>49.25</v>
+      </c>
+      <c r="M10" s="8">
+        <v>18055.72</v>
+      </c>
+      <c r="N10" s="8">
+        <v>8717.390000000001</v>
+      </c>
+      <c r="O10" s="8">
+        <v>9338.33</v>
+      </c>
+      <c r="P10" s="8">
+        <v>161.1043142</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" s="6"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" s="7">
+        <v>66.9909</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="G11" s="7">
+        <v>65.6097</v>
+      </c>
+      <c r="H11" s="11">
+        <v>1.31</v>
+      </c>
+      <c r="I11" s="8">
+        <v>131</v>
+      </c>
+      <c r="J11" s="8">
+        <v>8594.870000000001</v>
+      </c>
+      <c r="K11" s="11">
+        <v>1.0938</v>
+      </c>
+      <c r="L11" s="8">
+        <v>73.27</v>
+      </c>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12" s="12">
+        <v>100</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E12" s="4">
+        <v>69.57250000000001</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G12" s="4">
+        <v>69.61799999999999</v>
+      </c>
+      <c r="H12" s="13">
+        <v>4.54</v>
+      </c>
+      <c r="I12" s="5">
+        <v>454</v>
+      </c>
+      <c r="J12" s="5">
+        <v>31606.57</v>
+      </c>
+      <c r="K12" s="13">
+        <v>1.1058334</v>
+      </c>
+      <c r="L12" s="5">
+        <v>76.94</v>
+      </c>
+      <c r="M12" s="5">
+        <v>31606.57</v>
+      </c>
+      <c r="N12" s="5">
+        <v>76.94</v>
+      </c>
+      <c r="O12" s="5">
+        <v>31529.63</v>
+      </c>
+      <c r="P12" s="5">
+        <v>452.8941666</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" s="3"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="4">
+        <v>71.59739999999999</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G13" s="4">
+        <v>70.96299999999999</v>
+      </c>
+      <c r="H13" s="13">
+        <v>0</v>
+      </c>
+      <c r="I13" s="5">
+        <v>0</v>
+      </c>
+      <c r="J13" s="5">
+        <v>0</v>
+      </c>
+      <c r="K13" s="13">
+        <v>0</v>
+      </c>
+      <c r="L13" s="5">
+        <v>0</v>
+      </c>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="L14" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="M14" s="9">
+        <f>SUM(M10:M13)</f>
+        <v>0</v>
+      </c>
+      <c r="N14" s="9">
+        <f>SUM(N10:N13)</f>
+        <v>0</v>
+      </c>
+      <c r="O14" s="9">
+        <f>SUM(O10:O13)</f>
+        <v>0</v>
+      </c>
+      <c r="P14" s="9">
+        <f>SUM(P10:P13)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="M10:M11"/>
+    <mergeCell ref="N10:N11"/>
+    <mergeCell ref="O10:O11"/>
+    <mergeCell ref="P10:P11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="M12:M13"/>
+    <mergeCell ref="N12:N13"/>
+    <mergeCell ref="O12:O13"/>
+    <mergeCell ref="P12:P13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E14"/>
   <sheetViews>
@@ -1567,7 +1756,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1592,19 +1781,19 @@
     </row>
     <row r="8" spans="1:5" ht="60" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1626,13 +1815,13 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="3" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B10" s="5">
         <v>6.5</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D10" s="4">
         <v>77.2774</v>
@@ -1643,13 +1832,13 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="6" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B11" s="8">
         <v>10</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D11" s="7">
         <v>79.3323</v>
@@ -1660,13 +1849,13 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="3" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B12" s="5">
         <v>0.1</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="D12" s="4">
         <v>73.42610000000001</v>
@@ -1677,13 +1866,13 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="6" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B13" s="8">
         <v>-0.1</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="D13" s="7">
         <v>73.42610000000001</v>
@@ -1706,7 +1895,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L12"/>
   <sheetViews>
@@ -1730,7 +1919,7 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -1755,7 +1944,7 @@
     </row>
     <row r="8" spans="1:12" ht="60" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>42</v>
@@ -1831,13 +2020,13 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D10" s="4">
         <v>50</v>
@@ -1846,7 +2035,7 @@
         <v>72.9272</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="G10" s="4">
         <v>73.4453</v>
@@ -1869,13 +2058,13 @@
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="3" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -1889,13 +2078,13 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="3" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D12" s="4">
         <v>50</v>
@@ -1904,7 +2093,7 @@
         <v>70.4413</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="G12" s="4">
         <v>70.4999</v>

</xml_diff>